<commit_message>
modify AIC tables for aesthetics; estimate change in sponge richness between first and second parts of monitoring period
</commit_message>
<xml_diff>
--- a/Results_May_15_mostrecentupdateAugust3/combined_all_Current_Thesis.xlsx
+++ b/Results_May_15_mostrecentupdateAugust3/combined_all_Current_Thesis.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="24" windowWidth="14340" windowHeight="9288"/>
+    <workbookView xWindow="384" yWindow="24" windowWidth="14340" windowHeight="9288" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="combined_all" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>K</t>
   </si>
@@ -104,6 +105,21 @@
   </si>
   <si>
     <t>Model Names</t>
+  </si>
+  <si>
+    <t>Model Name</t>
+  </si>
+  <si>
+    <t>K*</t>
+  </si>
+  <si>
+    <t>Delta AICc</t>
+  </si>
+  <si>
+    <t>Akaike weight</t>
+  </si>
+  <si>
+    <t>Log-likelihood</t>
   </si>
 </sst>
 </file>
@@ -113,7 +129,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,8 +278,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,8 +472,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -585,6 +614,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -630,7 +670,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -639,6 +679,9 @@
     <xf numFmtId="2" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="19" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -983,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="A1:H23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1601,4 +1644,479 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1071.2980638017</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.97539934617151403</v>
+      </c>
+      <c r="F2" s="6">
+        <v>-523.78061084821798</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1079.7264395971799</v>
+      </c>
+      <c r="D3" s="6">
+        <v>8.4283757954835892</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1.4420619256530501E-2</v>
+      </c>
+      <c r="F3" s="6">
+        <v>-527.99479874596</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1083.03578485923</v>
+      </c>
+      <c r="D4" s="6">
+        <v>11.737721057535101</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2.7565680454345498E-3</v>
+      </c>
+      <c r="F4" s="6">
+        <v>-530.79893818125095</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1083.1092886142701</v>
+      </c>
+      <c r="D5" s="6">
+        <v>11.811224812568099</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2.6570980448317799E-3</v>
+      </c>
+      <c r="F5" s="6">
+        <v>-530.83569005876802</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1084.5200970639501</v>
+      </c>
+      <c r="D6" s="6">
+        <v>13.222033262252801</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.3123643290934401E-3</v>
+      </c>
+      <c r="F6" s="6">
+        <v>-530.39162747934495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1084.7855057358099</v>
+      </c>
+      <c r="D7" s="6">
+        <v>13.487441934113299</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.1492689055438701E-3</v>
+      </c>
+      <c r="F7" s="6">
+        <v>-523.29686245694802</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1084.83433853012</v>
+      </c>
+      <c r="D8" s="6">
+        <v>13.536274728424599</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.1215477026341599E-3</v>
+      </c>
+      <c r="F8" s="6">
+        <v>-532.83275368064596</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1086.0043008365001</v>
+      </c>
+      <c r="D9" s="6">
+        <v>14.7062370347985</v>
+      </c>
+      <c r="E9" s="4">
+        <v>6.2483257543122803E-4</v>
+      </c>
+      <c r="F9" s="6">
+        <v>-532.28319616988301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1086.4805882312601</v>
+      </c>
+      <c r="D10" s="6">
+        <v>15.1825244295605</v>
+      </c>
+      <c r="E10" s="4">
+        <v>4.92423952321386E-4</v>
+      </c>
+      <c r="F10" s="6">
+        <v>-532.52133986726403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1092.8367626306699</v>
+      </c>
+      <c r="D11" s="6">
+        <v>21.538698828968101</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2.0516980030227301E-5</v>
+      </c>
+      <c r="F11" s="6">
+        <v>-542.29259515181195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1093.2269530757601</v>
+      </c>
+      <c r="D12" s="6">
+        <v>21.928889274065298</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1.6880474769151999E-5</v>
+      </c>
+      <c r="F12" s="6">
+        <v>-527.51758612692402</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>17</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1093.2573845326301</v>
+      </c>
+      <c r="D13" s="6">
+        <v>21.9593207309292</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.6625570246166101E-5</v>
+      </c>
+      <c r="F13" s="6">
+        <v>-527.53280185535596</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2">
+        <v>5</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1094.8284644072401</v>
+      </c>
+      <c r="D14" s="6">
+        <v>23.5304006055385</v>
+      </c>
+      <c r="E14" s="4">
+        <v>7.5791567682372896E-6</v>
+      </c>
+      <c r="F14" s="6">
+        <v>-542.22435878589704</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2">
+        <v>17</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1096.1708425893801</v>
+      </c>
+      <c r="D15" s="6">
+        <v>24.872778787677099</v>
+      </c>
+      <c r="E15" s="4">
+        <v>3.8737105963424196E-6</v>
+      </c>
+      <c r="F15" s="6">
+        <v>-528.989530883729</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1101.1446470332401</v>
+      </c>
+      <c r="D16" s="6">
+        <v>29.846583231541199</v>
+      </c>
+      <c r="E16" s="4">
+        <v>3.2216566961740199E-7</v>
+      </c>
+      <c r="F16" s="6">
+        <v>-546.44653735309805</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1103.23423874727</v>
+      </c>
+      <c r="D17" s="6">
+        <v>31.936174945571999</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.13326162868782E-7</v>
+      </c>
+      <c r="F17" s="6">
+        <v>-546.42724595591403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1106.7570899441801</v>
+      </c>
+      <c r="D18" s="6">
+        <v>35.459026142484397</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.94694089055238E-8</v>
+      </c>
+      <c r="F18" s="6">
+        <v>-550.30354497209203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1116.3226185344199</v>
+      </c>
+      <c r="D19" s="6">
+        <v>45.024554732716503</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1.63013895158646E-10</v>
+      </c>
+      <c r="F19" s="6">
+        <v>-555.08630926720798</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1150.3694659058899</v>
+      </c>
+      <c r="D20" s="6">
+        <v>79.071402104193794</v>
+      </c>
+      <c r="E20" s="4">
+        <v>6.5924319428482502E-18</v>
+      </c>
+      <c r="F20" s="6">
+        <v>-572.10973295294696</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>4</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1151.50874465994</v>
+      </c>
+      <c r="D21" s="6">
+        <v>80.210680858242796</v>
+      </c>
+      <c r="E21" s="4">
+        <v>3.7295326792664502E-18</v>
+      </c>
+      <c r="F21" s="6">
+        <v>-571.62858616644905</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>5</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1152.67724919578</v>
+      </c>
+      <c r="D22" s="6">
+        <v>81.3791853940793</v>
+      </c>
+      <c r="E22" s="4">
+        <v>2.0792986946544199E-18</v>
+      </c>
+      <c r="F22" s="6">
+        <v>-571.14875118016801</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3">
+        <v>3</v>
+      </c>
+      <c r="C23" s="7">
+        <v>1153.81752666292</v>
+      </c>
+      <c r="D23" s="7">
+        <v>82.519462861223204</v>
+      </c>
+      <c r="E23" s="5">
+        <v>1.17573318150266E-18</v>
+      </c>
+      <c r="F23" s="7">
+        <v>-573.833763331461</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>